<commit_message>
Now building again nicely.
</commit_message>
<xml_diff>
--- a/Spreadsheets/Parts.xlsx
+++ b/Spreadsheets/Parts.xlsx
@@ -2647,6 +2647,24 @@
     <xf numFmtId="0" fontId="20" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -2664,24 +2682,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -3765,9 +3765,9 @@
   <dimension ref="A1:Y170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="I133" sqref="I133"/>
+      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3928,7 +3928,7 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="186" t="s">
+      <c r="A3" s="180" t="s">
         <v>134</v>
       </c>
       <c r="B3" s="174"/>
@@ -3956,7 +3956,7 @@
       <c r="V3" s="22"/>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="187"/>
+      <c r="A4" s="181"/>
       <c r="B4" s="174"/>
       <c r="C4" s="167"/>
       <c r="D4" s="57"/>
@@ -3982,7 +3982,7 @@
       <c r="V4" s="22"/>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="187"/>
+      <c r="A5" s="181"/>
       <c r="B5" s="174"/>
       <c r="C5" s="167"/>
       <c r="D5" s="57" t="s">
@@ -4014,7 +4014,7 @@
       <c r="V5" s="22"/>
     </row>
     <row r="6" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="187"/>
+      <c r="A6" s="181"/>
       <c r="B6" s="174"/>
       <c r="C6" s="167"/>
       <c r="D6" s="57" t="s">
@@ -4046,7 +4046,7 @@
       <c r="V6" s="22"/>
     </row>
     <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="187"/>
+      <c r="A7" s="181"/>
       <c r="B7" s="174"/>
       <c r="C7" s="167"/>
       <c r="D7" s="57" t="s">
@@ -4076,7 +4076,7 @@
       <c r="V7" s="22"/>
     </row>
     <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="187"/>
+      <c r="A8" s="181"/>
       <c r="B8" s="174"/>
       <c r="C8" s="167"/>
       <c r="D8" s="57" t="s">
@@ -4104,7 +4104,7 @@
       <c r="V8" s="22"/>
     </row>
     <row r="9" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="188"/>
+      <c r="A9" s="182"/>
       <c r="B9" s="174"/>
       <c r="C9" s="167"/>
       <c r="D9" s="57" t="s">
@@ -4184,7 +4184,7 @@
       <c r="V10" s="22"/>
     </row>
     <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="186" t="s">
+      <c r="A11" s="180" t="s">
         <v>95</v>
       </c>
       <c r="B11" s="174"/>
@@ -4219,7 +4219,7 @@
       <c r="V11" s="22"/>
     </row>
     <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="187"/>
+      <c r="A12" s="181"/>
       <c r="B12" s="174"/>
       <c r="C12" s="167"/>
       <c r="D12" s="43" t="s">
@@ -4250,7 +4250,7 @@
       <c r="V12" s="22"/>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="188"/>
+      <c r="A13" s="182"/>
       <c r="B13" s="174"/>
       <c r="C13" s="167"/>
       <c r="D13" s="43" t="s">
@@ -4374,7 +4374,7 @@
       <c r="V16" s="22"/>
     </row>
     <row r="17" spans="1:25" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="186" t="s">
+      <c r="A17" s="180" t="s">
         <v>94</v>
       </c>
       <c r="B17" s="174"/>
@@ -4419,7 +4419,7 @@
       <c r="V17" s="22"/>
     </row>
     <row r="18" spans="1:25" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="187"/>
+      <c r="A18" s="181"/>
       <c r="B18" s="174"/>
       <c r="C18" s="167"/>
       <c r="D18" s="43" t="s">
@@ -4462,7 +4462,7 @@
       <c r="V18" s="22"/>
     </row>
     <row r="19" spans="1:25" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="187"/>
+      <c r="A19" s="181"/>
       <c r="B19" s="174"/>
       <c r="C19" s="169"/>
       <c r="D19" s="43" t="s">
@@ -4507,7 +4507,7 @@
       <c r="V19" s="22"/>
     </row>
     <row r="20" spans="1:25" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="188"/>
+      <c r="A20" s="182"/>
       <c r="B20" s="174"/>
       <c r="C20" s="167"/>
       <c r="D20" s="43" t="s">
@@ -4600,7 +4600,7 @@
       <c r="V22" s="22"/>
     </row>
     <row r="23" spans="1:25" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="186" t="s">
+      <c r="A23" s="180" t="s">
         <v>99</v>
       </c>
       <c r="B23" s="174"/>
@@ -4649,7 +4649,7 @@
       <c r="V23" s="22"/>
     </row>
     <row r="24" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="187"/>
+      <c r="A24" s="181"/>
       <c r="B24" s="174"/>
       <c r="C24" s="169"/>
       <c r="D24" s="43" t="s">
@@ -4692,7 +4692,7 @@
       <c r="V24" s="22"/>
     </row>
     <row r="25" spans="1:25" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="187"/>
+      <c r="A25" s="181"/>
       <c r="B25" s="174"/>
       <c r="C25" s="169"/>
       <c r="D25" s="43" t="s">
@@ -4736,7 +4736,7 @@
       <c r="Y25" s="55"/>
     </row>
     <row r="26" spans="1:25" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="187"/>
+      <c r="A26" s="181"/>
       <c r="B26" s="174"/>
       <c r="C26" s="167"/>
       <c r="D26" s="43" t="s">
@@ -4779,7 +4779,7 @@
       <c r="V26" s="22"/>
     </row>
     <row r="27" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="187"/>
+      <c r="A27" s="181"/>
       <c r="B27" s="174"/>
       <c r="C27" s="170"/>
       <c r="D27" s="43" t="s">
@@ -4816,7 +4816,7 @@
       <c r="V27" s="22"/>
     </row>
     <row r="28" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="187"/>
+      <c r="A28" s="181"/>
       <c r="B28" s="174"/>
       <c r="C28" s="170"/>
       <c r="D28" s="43" t="s">
@@ -4853,7 +4853,7 @@
       <c r="V28" s="22"/>
     </row>
     <row r="29" spans="1:25" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="187"/>
+      <c r="A29" s="181"/>
       <c r="B29" s="174"/>
       <c r="C29" s="169"/>
       <c r="D29" s="43" t="s">
@@ -4894,7 +4894,7 @@
       <c r="V29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="187"/>
+      <c r="A30" s="181"/>
       <c r="B30" s="174"/>
       <c r="C30" s="167"/>
       <c r="D30" s="43" t="s">
@@ -4935,7 +4935,7 @@
       <c r="V30" s="22"/>
     </row>
     <row r="31" spans="1:25" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="188"/>
+      <c r="A31" s="182"/>
       <c r="B31" s="174"/>
       <c r="C31" s="167"/>
       <c r="D31" s="43" t="s">
@@ -4974,7 +4974,7 @@
       <c r="V31" s="22"/>
     </row>
     <row r="32" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="189" t="s">
+      <c r="A32" s="183" t="s">
         <v>98</v>
       </c>
       <c r="B32" s="175"/>
@@ -5031,7 +5031,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="190"/>
+      <c r="A33" s="184"/>
       <c r="B33" s="175"/>
       <c r="C33" s="167"/>
       <c r="D33" s="43" t="s">
@@ -5062,7 +5062,7 @@
       <c r="V33" s="22"/>
     </row>
     <row r="34" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="190"/>
+      <c r="A34" s="184"/>
       <c r="B34" s="175"/>
       <c r="C34" s="167"/>
       <c r="D34" s="43" t="s">
@@ -5093,7 +5093,7 @@
       <c r="V34" s="22"/>
     </row>
     <row r="35" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="190"/>
+      <c r="A35" s="184"/>
       <c r="B35" s="175"/>
       <c r="C35" s="167"/>
       <c r="D35" s="43" t="s">
@@ -5126,7 +5126,7 @@
       <c r="V35" s="22"/>
     </row>
     <row r="36" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="190"/>
+      <c r="A36" s="184"/>
       <c r="B36" s="175"/>
       <c r="C36" s="171"/>
       <c r="D36" s="43" t="s">
@@ -5165,7 +5165,7 @@
       <c r="V36" s="22"/>
     </row>
     <row r="37" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="190"/>
+      <c r="A37" s="184"/>
       <c r="B37" s="175"/>
       <c r="C37" s="167"/>
       <c r="D37" s="43" t="s">
@@ -5200,7 +5200,7 @@
       <c r="V37" s="22"/>
     </row>
     <row r="38" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="190"/>
+      <c r="A38" s="184"/>
       <c r="B38" s="175"/>
       <c r="C38" s="167"/>
       <c r="D38" s="80" t="s">
@@ -5232,7 +5232,7 @@
       <c r="V38" s="22"/>
     </row>
     <row r="39" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="191"/>
+      <c r="A39" s="185"/>
       <c r="B39" s="175"/>
       <c r="C39" s="167"/>
       <c r="D39" s="43"/>
@@ -5261,7 +5261,7 @@
       <c r="V39" s="22"/>
     </row>
     <row r="40" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="186" t="s">
+      <c r="A40" s="180" t="s">
         <v>97</v>
       </c>
       <c r="B40" s="174"/>
@@ -5296,7 +5296,7 @@
       <c r="V40" s="22"/>
     </row>
     <row r="41" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="187"/>
+      <c r="A41" s="181"/>
       <c r="B41" s="174"/>
       <c r="C41" s="172"/>
       <c r="D41" s="43" t="s">
@@ -5335,7 +5335,7 @@
       <c r="V41" s="22"/>
     </row>
     <row r="42" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="187"/>
+      <c r="A42" s="181"/>
       <c r="B42" s="174"/>
       <c r="C42" s="167"/>
       <c r="D42" s="43" t="s">
@@ -5372,7 +5372,7 @@
       <c r="V42" s="22"/>
     </row>
     <row r="43" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="187"/>
+      <c r="A43" s="181"/>
       <c r="B43" s="174"/>
       <c r="C43" s="172"/>
       <c r="D43" s="43" t="s">
@@ -5409,7 +5409,7 @@
       <c r="V43" s="22"/>
     </row>
     <row r="44" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="187"/>
+      <c r="A44" s="181"/>
       <c r="B44" s="174"/>
       <c r="C44" s="167"/>
       <c r="D44" s="43"/>
@@ -5444,7 +5444,7 @@
       <c r="V44" s="22"/>
     </row>
     <row r="45" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="187"/>
+      <c r="A45" s="181"/>
       <c r="B45" s="174"/>
       <c r="C45" s="167"/>
       <c r="D45" s="43" t="s">
@@ -5479,7 +5479,7 @@
       <c r="V45" s="22"/>
     </row>
     <row r="46" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="187"/>
+      <c r="A46" s="181"/>
       <c r="B46" s="174"/>
       <c r="C46" s="167"/>
       <c r="D46" s="154" t="s">
@@ -5522,7 +5522,7 @@
       <c r="V46" s="22"/>
     </row>
     <row r="47" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="188"/>
+      <c r="A47" s="182"/>
       <c r="B47" s="174"/>
       <c r="C47" s="167"/>
       <c r="D47" s="43"/>
@@ -5551,7 +5551,7 @@
       <c r="V47" s="22"/>
     </row>
     <row r="48" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="186" t="s">
+      <c r="A48" s="180" t="s">
         <v>96</v>
       </c>
       <c r="B48" s="174"/>
@@ -5586,7 +5586,7 @@
       <c r="V48" s="22"/>
     </row>
     <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="187"/>
+      <c r="A49" s="181"/>
       <c r="B49" s="174"/>
       <c r="C49" s="167"/>
       <c r="D49" s="51" t="s">
@@ -5619,7 +5619,7 @@
       <c r="V49" s="22"/>
     </row>
     <row r="50" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="187"/>
+      <c r="A50" s="181"/>
       <c r="B50" s="174"/>
       <c r="C50" s="167"/>
       <c r="D50" s="80" t="s">
@@ -5656,7 +5656,7 @@
       <c r="V50" s="22"/>
     </row>
     <row r="51" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="187"/>
+      <c r="A51" s="181"/>
       <c r="B51" s="174"/>
       <c r="C51" s="167"/>
       <c r="D51" s="80" t="s">
@@ -5691,7 +5691,7 @@
       <c r="V51" s="22"/>
     </row>
     <row r="52" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="188"/>
+      <c r="A52" s="182"/>
       <c r="B52" s="174"/>
       <c r="C52" s="167"/>
       <c r="D52" s="51" t="s">
@@ -5852,7 +5852,7 @@
       <c r="V56" s="22"/>
     </row>
     <row r="57" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="183" t="s">
+      <c r="A57" s="189" t="s">
         <v>272</v>
       </c>
       <c r="B57" s="176"/>
@@ -5885,7 +5885,7 @@
       <c r="V57" s="22"/>
     </row>
     <row r="58" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="184"/>
+      <c r="A58" s="190"/>
       <c r="B58" s="176"/>
       <c r="C58" s="167"/>
       <c r="D58" s="43" t="s">
@@ -5916,7 +5916,7 @@
       <c r="V58" s="22"/>
     </row>
     <row r="59" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="185"/>
+      <c r="A59" s="191"/>
       <c r="B59" s="176"/>
       <c r="C59" s="167"/>
       <c r="D59" s="43" t="s">
@@ -5976,7 +5976,7 @@
       <c r="V60" s="22"/>
     </row>
     <row r="61" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="180" t="s">
+      <c r="A61" s="186" t="s">
         <v>274</v>
       </c>
       <c r="B61" s="177" t="s">
@@ -6025,7 +6025,7 @@
       <c r="V61" s="22"/>
     </row>
     <row r="62" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="181"/>
+      <c r="A62" s="187"/>
       <c r="B62" s="177" t="s">
         <v>454</v>
       </c>
@@ -6072,7 +6072,7 @@
       <c r="V62" s="22"/>
     </row>
     <row r="63" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="181"/>
+      <c r="A63" s="187"/>
       <c r="B63" s="177" t="s">
         <v>454</v>
       </c>
@@ -6125,7 +6125,7 @@
       <c r="V63" s="22"/>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A64" s="181"/>
+      <c r="A64" s="187"/>
       <c r="B64" s="177" t="s">
         <v>454</v>
       </c>
@@ -6178,7 +6178,7 @@
       <c r="V64" s="22"/>
     </row>
     <row r="65" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="180" t="s">
+      <c r="A65" s="186" t="s">
         <v>275</v>
       </c>
       <c r="B65" s="177" t="s">
@@ -6227,7 +6227,7 @@
       <c r="V65" s="22"/>
     </row>
     <row r="66" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="181"/>
+      <c r="A66" s="187"/>
       <c r="B66" s="177" t="s">
         <v>454</v>
       </c>
@@ -6274,7 +6274,7 @@
       <c r="V66" s="22"/>
     </row>
     <row r="67" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="181"/>
+      <c r="A67" s="187"/>
       <c r="B67" s="177" t="s">
         <v>454</v>
       </c>
@@ -6327,7 +6327,7 @@
       <c r="V67" s="22"/>
     </row>
     <row r="68" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="181"/>
+      <c r="A68" s="187"/>
       <c r="B68" s="177" t="s">
         <v>454</v>
       </c>
@@ -6380,7 +6380,7 @@
       <c r="V68" s="22"/>
     </row>
     <row r="69" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="180" t="s">
+      <c r="A69" s="186" t="s">
         <v>276</v>
       </c>
       <c r="B69" s="177" t="s">
@@ -6429,7 +6429,7 @@
       <c r="V69" s="22"/>
     </row>
     <row r="70" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="181"/>
+      <c r="A70" s="187"/>
       <c r="B70" s="177" t="s">
         <v>454</v>
       </c>
@@ -6476,7 +6476,7 @@
       <c r="V70" s="22"/>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A71" s="181"/>
+      <c r="A71" s="187"/>
       <c r="B71" s="177" t="s">
         <v>454</v>
       </c>
@@ -6529,7 +6529,7 @@
       <c r="V71" s="22"/>
     </row>
     <row r="72" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="181"/>
+      <c r="A72" s="187"/>
       <c r="B72" s="177" t="s">
         <v>454</v>
       </c>
@@ -6582,7 +6582,7 @@
       <c r="V72" s="22"/>
     </row>
     <row r="73" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="180" t="s">
+      <c r="A73" s="186" t="s">
         <v>403</v>
       </c>
       <c r="B73" s="177" t="s">
@@ -6631,7 +6631,7 @@
       <c r="V73" s="22"/>
     </row>
     <row r="74" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="181"/>
+      <c r="A74" s="187"/>
       <c r="B74" s="177" t="s">
         <v>454</v>
       </c>
@@ -6678,7 +6678,7 @@
       <c r="V74" s="22"/>
     </row>
     <row r="75" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A75" s="181"/>
+      <c r="A75" s="187"/>
       <c r="B75" s="177" t="s">
         <v>454</v>
       </c>
@@ -6731,7 +6731,7 @@
       <c r="V75" s="22"/>
     </row>
     <row r="76" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="182"/>
+      <c r="A76" s="188"/>
       <c r="B76" s="177" t="s">
         <v>454</v>
       </c>
@@ -6784,7 +6784,7 @@
       <c r="V76" s="22"/>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A77" s="180" t="s">
+      <c r="A77" s="186" t="s">
         <v>277</v>
       </c>
       <c r="B77" s="177" t="s">
@@ -6841,7 +6841,7 @@
       <c r="V77" s="22"/>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A78" s="181"/>
+      <c r="A78" s="187"/>
       <c r="B78" s="177" t="s">
         <v>454</v>
       </c>
@@ -6896,7 +6896,7 @@
       <c r="V78" s="22"/>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A79" s="182"/>
+      <c r="A79" s="188"/>
       <c r="B79" s="177" t="s">
         <v>454</v>
       </c>
@@ -6951,7 +6951,7 @@
       <c r="V79" s="22"/>
     </row>
     <row r="80" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="180" t="s">
+      <c r="A80" s="186" t="s">
         <v>278</v>
       </c>
       <c r="B80" s="177" t="s">
@@ -6998,7 +6998,7 @@
       <c r="V80" s="22"/>
     </row>
     <row r="81" spans="1:22" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="182"/>
+      <c r="A81" s="188"/>
       <c r="B81" s="177"/>
       <c r="C81" s="167"/>
       <c r="D81" s="43"/>
@@ -7025,7 +7025,7 @@
       <c r="V81" s="22"/>
     </row>
     <row r="82" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="180" t="s">
+      <c r="A82" s="186" t="s">
         <v>279</v>
       </c>
       <c r="B82" s="177" t="s">
@@ -7072,7 +7072,7 @@
       <c r="V82" s="22"/>
     </row>
     <row r="83" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="181"/>
+      <c r="A83" s="187"/>
       <c r="B83" s="177" t="s">
         <v>454</v>
       </c>
@@ -7119,7 +7119,7 @@
       <c r="V83" s="22"/>
     </row>
     <row r="84" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="181"/>
+      <c r="A84" s="187"/>
       <c r="B84" s="177" t="s">
         <v>454</v>
       </c>
@@ -7168,7 +7168,7 @@
       <c r="V84" s="22"/>
     </row>
     <row r="85" spans="1:22" s="152" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="181"/>
+      <c r="A85" s="187"/>
       <c r="B85" s="177" t="s">
         <v>454</v>
       </c>
@@ -7223,7 +7223,7 @@
       <c r="V85" s="22"/>
     </row>
     <row r="86" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="181"/>
+      <c r="A86" s="187"/>
       <c r="B86" s="177"/>
       <c r="C86" s="167"/>
       <c r="D86" s="51"/>
@@ -7247,7 +7247,7 @@
       <c r="V86" s="22"/>
     </row>
     <row r="87" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="181"/>
+      <c r="A87" s="187"/>
       <c r="B87" s="177" t="s">
         <v>454</v>
       </c>
@@ -7298,7 +7298,7 @@
       <c r="V87" s="22"/>
     </row>
     <row r="88" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="182"/>
+      <c r="A88" s="188"/>
       <c r="B88" s="177" t="s">
         <v>454</v>
       </c>
@@ -7355,7 +7355,7 @@
       <c r="V88" s="22"/>
     </row>
     <row r="89" spans="1:22" s="152" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="180" t="s">
+      <c r="A89" s="186" t="s">
         <v>280</v>
       </c>
       <c r="B89" s="177"/>
@@ -7386,7 +7386,7 @@
       <c r="V89" s="22"/>
     </row>
     <row r="90" spans="1:22" s="152" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="182"/>
+      <c r="A90" s="188"/>
       <c r="B90" s="177"/>
       <c r="C90" s="167"/>
       <c r="D90" s="43"/>
@@ -7415,7 +7415,7 @@
       <c r="V90" s="22"/>
     </row>
     <row r="91" spans="1:22" s="152" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="180" t="s">
+      <c r="A91" s="186" t="s">
         <v>281</v>
       </c>
       <c r="B91" s="177"/>
@@ -7446,7 +7446,7 @@
       <c r="V91" s="22"/>
     </row>
     <row r="92" spans="1:22" s="152" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="182"/>
+      <c r="A92" s="188"/>
       <c r="B92" s="177"/>
       <c r="C92" s="167"/>
       <c r="D92" s="43"/>
@@ -7475,7 +7475,7 @@
       <c r="V92" s="22"/>
     </row>
     <row r="93" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="180" t="s">
+      <c r="A93" s="186" t="s">
         <v>282</v>
       </c>
       <c r="B93" s="177" t="s">
@@ -7526,7 +7526,7 @@
       <c r="V93" s="22"/>
     </row>
     <row r="94" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="181"/>
+      <c r="A94" s="187"/>
       <c r="B94" s="177" t="s">
         <v>454</v>
       </c>
@@ -7577,7 +7577,7 @@
       <c r="V94" s="22"/>
     </row>
     <row r="95" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="181"/>
+      <c r="A95" s="187"/>
       <c r="B95" s="177" t="s">
         <v>454</v>
       </c>
@@ -7626,7 +7626,7 @@
       <c r="V95" s="22"/>
     </row>
     <row r="96" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="182"/>
+      <c r="A96" s="188"/>
       <c r="B96" s="177" t="s">
         <v>454</v>
       </c>
@@ -7675,7 +7675,7 @@
       <c r="V96" s="22"/>
     </row>
     <row r="97" spans="1:23" s="152" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="180" t="s">
+      <c r="A97" s="186" t="s">
         <v>283</v>
       </c>
       <c r="B97" s="177" t="s">
@@ -7732,7 +7732,7 @@
       <c r="V97" s="22"/>
     </row>
     <row r="98" spans="1:23" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="181"/>
+      <c r="A98" s="187"/>
       <c r="B98" s="177" t="s">
         <v>454</v>
       </c>
@@ -7787,7 +7787,7 @@
       <c r="V98" s="22"/>
     </row>
     <row r="99" spans="1:23" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="181"/>
+      <c r="A99" s="187"/>
       <c r="B99" s="177" t="s">
         <v>454</v>
       </c>
@@ -7842,7 +7842,7 @@
       <c r="V99" s="22"/>
     </row>
     <row r="100" spans="1:23" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="182"/>
+      <c r="A100" s="188"/>
       <c r="B100" s="177" t="s">
         <v>454</v>
       </c>
@@ -7897,7 +7897,7 @@
       <c r="V100" s="22"/>
     </row>
     <row r="101" spans="1:23" s="152" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="180" t="s">
+      <c r="A101" s="186" t="s">
         <v>358</v>
       </c>
       <c r="B101" s="177" t="s">
@@ -7945,7 +7945,7 @@
       <c r="W101" s="1"/>
     </row>
     <row r="102" spans="1:23" s="152" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="181"/>
+      <c r="A102" s="187"/>
       <c r="B102" s="177" t="s">
         <v>454</v>
       </c>
@@ -7988,7 +7988,7 @@
       <c r="V102" s="22"/>
     </row>
     <row r="103" spans="1:23" s="152" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="181"/>
+      <c r="A103" s="187"/>
       <c r="B103" s="177" t="s">
         <v>454</v>
       </c>
@@ -8039,7 +8039,7 @@
       <c r="V103" s="22"/>
     </row>
     <row r="104" spans="1:23" s="152" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="181"/>
+      <c r="A104" s="187"/>
       <c r="B104" s="177" t="s">
         <v>454</v>
       </c>
@@ -8088,7 +8088,7 @@
       <c r="V104" s="22"/>
     </row>
     <row r="105" spans="1:23" s="152" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="181"/>
+      <c r="A105" s="187"/>
       <c r="B105" s="177" t="s">
         <v>454</v>
       </c>
@@ -8135,7 +8135,7 @@
       <c r="V105" s="22"/>
     </row>
     <row r="106" spans="1:23" s="152" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="181"/>
+      <c r="A106" s="187"/>
       <c r="B106" s="177" t="s">
         <v>454</v>
       </c>
@@ -8190,7 +8190,7 @@
       <c r="V106" s="22"/>
     </row>
     <row r="107" spans="1:23" s="152" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="181"/>
+      <c r="A107" s="187"/>
       <c r="B107" s="177"/>
       <c r="C107" s="167"/>
       <c r="D107" s="51" t="s">
@@ -8243,7 +8243,7 @@
       <c r="V107" s="22"/>
     </row>
     <row r="108" spans="1:23" s="152" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="181"/>
+      <c r="A108" s="187"/>
       <c r="B108" s="177" t="s">
         <v>454</v>
       </c>
@@ -8292,7 +8292,7 @@
       <c r="V108" s="22"/>
     </row>
     <row r="109" spans="1:23" s="152" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="181"/>
+      <c r="A109" s="187"/>
       <c r="B109" s="177"/>
       <c r="C109" s="167"/>
       <c r="D109" s="51" t="s">
@@ -8339,7 +8339,7 @@
       <c r="V109" s="22"/>
     </row>
     <row r="110" spans="1:23" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="181"/>
+      <c r="A110" s="187"/>
       <c r="B110" s="177"/>
       <c r="C110" s="167"/>
       <c r="D110" s="51" t="s">
@@ -8386,7 +8386,7 @@
       <c r="V110" s="22"/>
     </row>
     <row r="111" spans="1:23" s="152" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="181"/>
+      <c r="A111" s="187"/>
       <c r="B111" s="177" t="s">
         <v>454</v>
       </c>
@@ -8439,7 +8439,7 @@
       <c r="V111" s="22"/>
     </row>
     <row r="112" spans="1:23" s="152" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="182"/>
+      <c r="A112" s="188"/>
       <c r="B112" s="177" t="s">
         <v>454</v>
       </c>
@@ -8488,7 +8488,7 @@
       <c r="V112" s="22"/>
     </row>
     <row r="113" spans="1:22" s="152" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="180" t="s">
+      <c r="A113" s="186" t="s">
         <v>439</v>
       </c>
       <c r="B113" s="177" t="s">
@@ -8545,7 +8545,7 @@
       <c r="V113" s="22"/>
     </row>
     <row r="114" spans="1:22" s="152" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="181"/>
+      <c r="A114" s="187"/>
       <c r="B114" s="177"/>
       <c r="C114" s="167"/>
       <c r="D114" s="51" t="s">
@@ -8598,7 +8598,7 @@
       <c r="V114" s="22"/>
     </row>
     <row r="115" spans="1:22" s="152" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="181"/>
+      <c r="A115" s="187"/>
       <c r="B115" s="177" t="s">
         <v>454</v>
       </c>
@@ -8653,7 +8653,7 @@
       <c r="V115" s="22"/>
     </row>
     <row r="116" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="182"/>
+      <c r="A116" s="188"/>
       <c r="B116" s="177" t="s">
         <v>454</v>
       </c>
@@ -8708,7 +8708,7 @@
       <c r="V116" s="22"/>
     </row>
     <row r="117" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="180" t="s">
+      <c r="A117" s="186" t="s">
         <v>284</v>
       </c>
       <c r="B117" s="177" t="s">
@@ -8757,7 +8757,7 @@
       <c r="V117" s="22"/>
     </row>
     <row r="118" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="181"/>
+      <c r="A118" s="187"/>
       <c r="B118" s="177" t="s">
         <v>454</v>
       </c>
@@ -8804,7 +8804,7 @@
       <c r="V118" s="22"/>
     </row>
     <row r="119" spans="1:22" s="152" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="181"/>
+      <c r="A119" s="187"/>
       <c r="B119" s="177" t="s">
         <v>454</v>
       </c>
@@ -8851,7 +8851,7 @@
       <c r="V119" s="22"/>
     </row>
     <row r="120" spans="1:22" s="152" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="181"/>
+      <c r="A120" s="187"/>
       <c r="B120" s="177"/>
       <c r="C120" s="167"/>
       <c r="D120" s="51" t="s">
@@ -8896,7 +8896,7 @@
       <c r="V120" s="22"/>
     </row>
     <row r="121" spans="1:22" s="152" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="181"/>
+      <c r="A121" s="187"/>
       <c r="B121" s="177" t="s">
         <v>454</v>
       </c>
@@ -8949,7 +8949,7 @@
       <c r="V121" s="22"/>
     </row>
     <row r="122" spans="1:22" s="152" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="182"/>
+      <c r="A122" s="188"/>
       <c r="B122" s="177" t="s">
         <v>454</v>
       </c>
@@ -10379,13 +10379,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A23:A31"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="A32:A39"/>
     <mergeCell ref="A101:A112"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="A117:A122"/>
@@ -10401,6 +10394,13 @@
     <mergeCell ref="A73:A76"/>
     <mergeCell ref="A113:A116"/>
     <mergeCell ref="A93:A96"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A23:A31"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="A32:A39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K36" r:id="rId1"/>
@@ -10594,7 +10594,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="180" t="s">
         <v>250</v>
       </c>
       <c r="B2" s="84"/>
@@ -10643,7 +10643,7 @@
       <c r="U2" s="22"/>
     </row>
     <row r="3" spans="1:21" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="187"/>
+      <c r="A3" s="181"/>
       <c r="B3" s="39"/>
       <c r="C3" s="43" t="s">
         <v>189</v>
@@ -10693,7 +10693,7 @@
       <c r="U3" s="22"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="187"/>
+      <c r="A4" s="181"/>
       <c r="B4" s="39"/>
       <c r="C4" s="51" t="s">
         <v>223</v>
@@ -10738,7 +10738,7 @@
       <c r="U4" s="22"/>
     </row>
     <row r="5" spans="1:21" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="187"/>
+      <c r="A5" s="181"/>
       <c r="B5" s="23"/>
       <c r="C5" s="43" t="s">
         <v>93</v>
@@ -10783,7 +10783,7 @@
       <c r="U5" s="22"/>
     </row>
     <row r="6" spans="1:21" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="187"/>
+      <c r="A6" s="181"/>
       <c r="B6" s="88"/>
       <c r="C6" s="43" t="s">
         <v>93</v>
@@ -10822,7 +10822,7 @@
       <c r="U6" s="22"/>
     </row>
     <row r="7" spans="1:21" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="187"/>
+      <c r="A7" s="181"/>
       <c r="B7" s="88"/>
       <c r="C7" s="43" t="s">
         <v>93</v>
@@ -10861,7 +10861,7 @@
       <c r="U7" s="22"/>
     </row>
     <row r="8" spans="1:21" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="187"/>
+      <c r="A8" s="181"/>
       <c r="B8" s="39"/>
       <c r="C8" s="43" t="s">
         <v>93</v>
@@ -10902,7 +10902,7 @@
       <c r="U8" s="22"/>
     </row>
     <row r="9" spans="1:21" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="187"/>
+      <c r="A9" s="181"/>
       <c r="B9" s="23"/>
       <c r="C9" s="43" t="s">
         <v>93</v>
@@ -10943,7 +10943,7 @@
       <c r="U9" s="22"/>
     </row>
     <row r="10" spans="1:21" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="188"/>
+      <c r="A10" s="182"/>
       <c r="B10" s="23"/>
       <c r="C10" s="43" t="s">
         <v>93</v>

</xml_diff>